<commit_message>
Addition of Task 2 Part A, B, C to validation
</commit_message>
<xml_diff>
--- a/REopt Julia Package Scripts/results/results_retire_existingboiler.xlsx
+++ b/REopt Julia Package Scripts/results/results_retire_existingboiler.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\REopt-Analysis-Scripts\REopt Julia Package Scripts\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\REopt-Analysis-Scripts\REopt Julia Package Scripts\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AB7D9A-5E43-4DC9-BF94-CE6CB9ECA0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE60B4C-8C63-49A9-BD16-DCE4DD237B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="results_0" sheetId="2" r:id="rId2"/>
     <sheet name="results_1" sheetId="3" r:id="rId3"/>
+    <sheet name="results_2" sheetId="4" r:id="rId4"/>
+    <sheet name="results_3" sheetId="5" r:id="rId5"/>
+    <sheet name="resultsB_0" sheetId="6" r:id="rId6"/>
+    <sheet name="resultsC_0" sheetId="7" r:id="rId7"/>
+    <sheet name="resultsB_1" sheetId="8" r:id="rId8"/>
+    <sheet name="resultsC_1" sheetId="9" r:id="rId9"/>
+    <sheet name="resultsB_2" sheetId="10" r:id="rId10"/>
+    <sheet name="resultsC_2" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="22">
   <si>
     <t>Region</t>
   </si>
@@ -68,13 +76,50 @@
   </si>
   <si>
     <t>West</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Total_Annual_Emissions_CO2</t>
+  </si>
+  <si>
+    <t>LifeCycle_Emissions_CO2</t>
+  </si>
+  <si>
+    <t>NG_LifeCycle_Emissions_CO2</t>
+  </si>
+  <si>
+    <t>LifeCycle_Emission_Reduction_Fraction</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>PV_size</t>
+  </si>
+  <si>
+    <t>Battery_size</t>
+  </si>
+  <si>
+    <t>npv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -102,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,17 +155,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,7 +468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DCE19F-6200-48CF-B18E-76732ABC5AD7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B8C142-C071-4502-8416-2DE670AE72A3}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -409,120 +479,391 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81ACF266-0B62-4A69-B067-F8AC3795F487}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>3067.76</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2471.17</v>
+      </c>
+      <c r="E2">
+        <v>61778.39</v>
+      </c>
+      <c r="F2">
+        <v>61773.68</v>
+      </c>
+      <c r="G2">
+        <v>0.24</v>
+      </c>
+      <c r="H2">
+        <v>-2741986.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2846.35</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2474.69</v>
+      </c>
+      <c r="E3">
+        <v>61778.39</v>
+      </c>
+      <c r="F3">
+        <v>61228.46</v>
+      </c>
+      <c r="G3">
+        <v>0.24</v>
+      </c>
+      <c r="H3">
+        <v>-2296535.7799999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2671.48</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2471.12</v>
+      </c>
+      <c r="E4">
+        <v>61778.400000000001</v>
+      </c>
+      <c r="F4">
+        <v>61780.37</v>
+      </c>
+      <c r="G4">
+        <v>0.24</v>
+      </c>
+      <c r="H4">
+        <v>-2543875.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>2471.4299999999998</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2471.14</v>
+      </c>
+      <c r="E5">
+        <v>61778.39</v>
+      </c>
+      <c r="F5">
+        <v>61778.38</v>
+      </c>
+      <c r="G5">
+        <v>0.24</v>
+      </c>
+      <c r="H5">
+        <v>-1937771.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE5EEF4-9E9C-4BDE-8BA5-F282C0B1C5DF}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>5971.42</v>
+      </c>
+      <c r="C2">
+        <v>6268.35</v>
+      </c>
+      <c r="D2">
+        <v>1950.91</v>
+      </c>
+      <c r="E2">
+        <v>48772.42</v>
+      </c>
+      <c r="F2">
+        <v>48769.599999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>9182.89</v>
+      </c>
+      <c r="C3">
+        <v>18729.080000000002</v>
+      </c>
+      <c r="D3">
+        <v>1300.6199999999999</v>
+      </c>
+      <c r="E3">
+        <v>32514.94</v>
+      </c>
+      <c r="F3">
+        <v>32512.02</v>
+      </c>
+      <c r="G3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>14311.35</v>
+      </c>
+      <c r="C4">
+        <v>29848.17</v>
+      </c>
+      <c r="D4">
+        <v>650.32000000000005</v>
+      </c>
+      <c r="E4">
+        <v>16257.47</v>
+      </c>
+      <c r="F4">
+        <v>16253.83</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>37354.019999999997</v>
+      </c>
+      <c r="C5">
+        <v>121192.39</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429A57D8-0DE0-4A92-A97E-F9755AA1CD59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8883EEAC-3FA4-4096-B437-04933A91825D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>3.3479999999999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>53868.05</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>20.350000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>68.819999999999993</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>417237.65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>3.3479999999999999</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>53868.05</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>24.47</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>82.75</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>490788.05</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3.3479999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>53868.05</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>17.63</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>59.62</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>368661.65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3.3479999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>53868.05</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>24.09</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>81.47</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>484029.65</v>
       </c>
     </row>
@@ -532,10 +873,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A191A1A-FC58-435C-8C72-B9E3F573DA70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E30D7B6-E1C0-49E5-8D42-130CD2A57371}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -644,4 +985,652 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDF1292-5C70-4131-859C-D54D94E7DC15}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C2">
+        <v>53860.32</v>
+      </c>
+      <c r="D2">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="E2">
+        <v>68.81</v>
+      </c>
+      <c r="F2">
+        <v>417177.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C3">
+        <v>53860.32</v>
+      </c>
+      <c r="D3">
+        <v>24.47</v>
+      </c>
+      <c r="E3">
+        <v>82.74</v>
+      </c>
+      <c r="F3">
+        <v>490727.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C4">
+        <v>53860.32</v>
+      </c>
+      <c r="D4">
+        <v>17.63</v>
+      </c>
+      <c r="E4">
+        <v>59.61</v>
+      </c>
+      <c r="F4">
+        <v>368601.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C5">
+        <v>53860.32</v>
+      </c>
+      <c r="D5">
+        <v>24.09</v>
+      </c>
+      <c r="E5">
+        <v>81.45</v>
+      </c>
+      <c r="F5">
+        <v>483916.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA2C0CE-D3B3-4FAB-A294-4E79BF0C1A13}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C2">
+        <v>53860.32</v>
+      </c>
+      <c r="D2">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="E2">
+        <v>68.81</v>
+      </c>
+      <c r="F2">
+        <v>417177.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C3">
+        <v>53860.32</v>
+      </c>
+      <c r="D3">
+        <v>24.47</v>
+      </c>
+      <c r="E3">
+        <v>82.74</v>
+      </c>
+      <c r="F3">
+        <v>490727.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C4">
+        <v>53860.32</v>
+      </c>
+      <c r="D4">
+        <v>17.63</v>
+      </c>
+      <c r="E4">
+        <v>59.61</v>
+      </c>
+      <c r="F4">
+        <v>368601.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3.3479999999999999</v>
+      </c>
+      <c r="C5">
+        <v>53860.32</v>
+      </c>
+      <c r="D5">
+        <v>24.09</v>
+      </c>
+      <c r="E5">
+        <v>81.45</v>
+      </c>
+      <c r="F5">
+        <v>483916.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5339081-82C1-4463-842C-6642C614D58A}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>2471.17</v>
+      </c>
+      <c r="C2">
+        <v>61778.39</v>
+      </c>
+      <c r="D2">
+        <v>61773.68</v>
+      </c>
+      <c r="E2">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2474.69</v>
+      </c>
+      <c r="C3">
+        <v>61778.39</v>
+      </c>
+      <c r="D3">
+        <v>61228.46</v>
+      </c>
+      <c r="E3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2471.12</v>
+      </c>
+      <c r="C4">
+        <v>61778.400000000001</v>
+      </c>
+      <c r="D4">
+        <v>61780.37</v>
+      </c>
+      <c r="E4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>2471.14</v>
+      </c>
+      <c r="C5">
+        <v>61778.39</v>
+      </c>
+      <c r="D5">
+        <v>61778.38</v>
+      </c>
+      <c r="E5">
+        <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128C31AF-1B1A-43A9-B54A-147F5A672126}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1950.91</v>
+      </c>
+      <c r="C2">
+        <v>48772.42</v>
+      </c>
+      <c r="D2">
+        <v>48769.599999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1300.6199999999999</v>
+      </c>
+      <c r="C3">
+        <v>32514.94</v>
+      </c>
+      <c r="D3">
+        <v>32512.02</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>650.32000000000005</v>
+      </c>
+      <c r="C4">
+        <v>16257.47</v>
+      </c>
+      <c r="D4">
+        <v>16253.83</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0D5B94-1456-47E3-9C0A-0D035CF93ADD}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>3067.76</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2471.17</v>
+      </c>
+      <c r="E2">
+        <v>61778.39</v>
+      </c>
+      <c r="F2">
+        <v>61773.68</v>
+      </c>
+      <c r="G2">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2846.35</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2474.69</v>
+      </c>
+      <c r="E3">
+        <v>61778.39</v>
+      </c>
+      <c r="F3">
+        <v>61228.46</v>
+      </c>
+      <c r="G3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2671.48</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2471.12</v>
+      </c>
+      <c r="E4">
+        <v>61778.400000000001</v>
+      </c>
+      <c r="F4">
+        <v>61780.37</v>
+      </c>
+      <c r="G4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>2471.4299999999998</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2471.14</v>
+      </c>
+      <c r="E5">
+        <v>61778.39</v>
+      </c>
+      <c r="F5">
+        <v>61778.38</v>
+      </c>
+      <c r="G5">
+        <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FDBA51-4230-4DDC-95D5-200CF78D8FCB}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1950.91</v>
+      </c>
+      <c r="C2">
+        <v>48772.42</v>
+      </c>
+      <c r="D2">
+        <v>48769.599999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1300.6199999999999</v>
+      </c>
+      <c r="C3">
+        <v>32514.94</v>
+      </c>
+      <c r="D3">
+        <v>32512.02</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>650.32000000000005</v>
+      </c>
+      <c r="C4">
+        <v>16257.47</v>
+      </c>
+      <c r="D4">
+        <v>16253.83</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>